<commit_message>
Total revamp of project
Moved from using JSON files to using a MONGO database for storing all
information from Excel files.

Created code for obtaining Altmetrics impact, and Scopus citations
</commit_message>
<xml_diff>
--- a/Data_files/affiliations.xlsx
+++ b/Data_files/affiliations.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amaral/PycharmProjects/maintaining_latex_cv/Data_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amaral/Box Sync/CodingProjects/maintaining_latex_cv/Data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753FB63A-1DF1-7A4D-974E-7D7946B44B5A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1500" windowWidth="27360" windowHeight="15880" tabRatio="500"/>
+    <workbookView xWindow="10020" yWindow="6200" windowWidth="27360" windowHeight="15880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Organization</t>
   </si>
@@ -87,12 +88,21 @@
   </si>
   <si>
     <t>http://siam.org/</t>
+  </si>
+  <si>
+    <t>Association for Information Science and Technology</t>
+  </si>
+  <si>
+    <t>Silver Spring, MD</t>
+  </si>
+  <si>
+    <t>https://www.asist.org/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -159,6 +169,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -426,11 +439,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -490,7 +503,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A6" si="0">A3+1</f>
+        <f t="shared" ref="A4:A7" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -543,7 +556,22 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>

</xml_diff>